<commit_message>
Ajout couleur pour membres / Tableau planning
</commit_message>
<xml_diff>
--- a/gestion-projet/Liste des taches.xlsx
+++ b/gestion-projet/Liste des taches.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15435" windowHeight="6585"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19965" windowHeight="8640"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="69">
   <si>
     <t>A faire</t>
   </si>
@@ -214,13 +215,22 @@
   </si>
   <si>
     <t>Tous</t>
+  </si>
+  <si>
+    <t>Florian</t>
+  </si>
+  <si>
+    <t>Melvin</t>
+  </si>
+  <si>
+    <t>Valentin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -270,7 +280,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -280,6 +290,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -311,7 +339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -333,12 +361,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,7 +432,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -431,9 +464,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -465,6 +499,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -640,17 +675,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H77"/>
+  <dimension ref="A1:J77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="56.85546875" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" style="2" customWidth="1"/>
@@ -660,20 +695,21 @@
     <col min="6" max="6" width="14" style="2" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" style="2" customWidth="1"/>
     <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="10" max="10" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-    </row>
-    <row r="2" spans="1:8" ht="17.25" customHeight="1">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+    </row>
+    <row r="2" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -682,18 +718,23 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:8" ht="18.75">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-    </row>
-    <row r="5" spans="1:8" ht="18.75">
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J4" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -718,13 +759,21 @@
       <c r="H5" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75">
+      <c r="J5" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J6" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -744,12 +793,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75">
+    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -769,12 +818,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.75">
+    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -794,12 +843,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15.75">
+    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -813,12 +862,12 @@
       <c r="G17" s="7"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="19" spans="1:8" ht="15.75">
+    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -838,7 +887,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -858,7 +907,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -872,7 +921,7 @@
       <c r="G22" s="7"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -886,7 +935,7 @@
       <c r="G23" s="7"/>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -900,7 +949,7 @@
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -920,7 +969,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -940,7 +989,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -954,7 +1003,7 @@
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -968,7 +1017,7 @@
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>23</v>
       </c>
@@ -982,7 +1031,7 @@
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -1002,7 +1051,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -1022,7 +1071,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>25</v>
       </c>
@@ -1040,7 +1089,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>26</v>
       </c>
@@ -1054,7 +1103,7 @@
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>27</v>
       </c>
@@ -1074,7 +1123,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>28</v>
       </c>
@@ -1088,7 +1137,7 @@
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>29</v>
       </c>
@@ -1102,7 +1151,7 @@
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>30</v>
       </c>
@@ -1116,7 +1165,7 @@
       <c r="G37" s="7"/>
       <c r="H37" s="5"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>31</v>
       </c>
@@ -1130,7 +1179,7 @@
       <c r="G38" s="7"/>
       <c r="H38" s="5"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>32</v>
       </c>
@@ -1144,7 +1193,7 @@
       <c r="G39" s="7"/>
       <c r="H39" s="5"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>33</v>
       </c>
@@ -1164,7 +1213,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="18.75">
+    <row r="43" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>42</v>
       </c>
@@ -1190,7 +1239,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>64</v>
       </c>
@@ -1206,7 +1255,7 @@
       <c r="G45" s="7"/>
       <c r="H45" s="5"/>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>43</v>
       </c>
@@ -1220,7 +1269,7 @@
       <c r="G47" s="7"/>
       <c r="H47" s="5"/>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>44</v>
       </c>
@@ -1234,16 +1283,16 @@
       <c r="G48" s="7"/>
       <c r="H48" s="5"/>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
       <c r="E49" s="8"/>
-      <c r="F49" s="10"/>
-      <c r="G49" s="10"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
       <c r="H49" s="8"/>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>45</v>
       </c>
@@ -1257,7 +1306,7 @@
       <c r="G50" s="7"/>
       <c r="H50" s="5"/>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>46</v>
       </c>
@@ -1271,16 +1320,16 @@
       <c r="G51" s="5"/>
       <c r="H51" s="5"/>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
       <c r="D52" s="8"/>
       <c r="E52" s="8"/>
       <c r="F52" s="8"/>
-      <c r="G52" s="10"/>
+      <c r="G52" s="9"/>
       <c r="H52" s="8"/>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>47</v>
       </c>
@@ -1294,7 +1343,7 @@
       <c r="G53" s="7"/>
       <c r="H53" s="5"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -1308,7 +1357,7 @@
       <c r="G54" s="5"/>
       <c r="H54" s="5"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B55" s="8"/>
       <c r="C55" s="8"/>
       <c r="D55" s="8"/>
@@ -1317,7 +1366,7 @@
       <c r="G55" s="8"/>
       <c r="H55" s="8"/>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>49</v>
       </c>
@@ -1337,7 +1386,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>50</v>
       </c>
@@ -1357,16 +1406,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B58" s="8"/>
       <c r="C58" s="8"/>
       <c r="D58" s="8"/>
       <c r="E58" s="8"/>
       <c r="F58" s="8"/>
-      <c r="G58" s="10"/>
+      <c r="G58" s="9"/>
       <c r="H58" s="8"/>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>51</v>
       </c>
@@ -1386,7 +1435,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>52</v>
       </c>
@@ -1406,16 +1455,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B61" s="8"/>
       <c r="C61" s="8"/>
       <c r="D61" s="8"/>
       <c r="E61" s="8"/>
       <c r="F61" s="8"/>
-      <c r="G61" s="10"/>
+      <c r="G61" s="9"/>
       <c r="H61" s="8"/>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>53</v>
       </c>
@@ -1429,7 +1478,7 @@
       <c r="G62" s="5"/>
       <c r="H62" s="5"/>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>54</v>
       </c>
@@ -1443,16 +1492,16 @@
       <c r="G63" s="5"/>
       <c r="H63" s="5"/>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B64" s="8"/>
       <c r="C64" s="8"/>
       <c r="D64" s="8"/>
       <c r="E64" s="8"/>
-      <c r="F64" s="10"/>
-      <c r="G64" s="10"/>
+      <c r="F64" s="9"/>
+      <c r="G64" s="9"/>
       <c r="H64" s="8"/>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>55</v>
       </c>
@@ -1472,7 +1521,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>56</v>
       </c>
@@ -1492,16 +1541,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
       <c r="D67" s="8"/>
       <c r="E67" s="8"/>
-      <c r="F67" s="10"/>
-      <c r="G67" s="10"/>
+      <c r="F67" s="9"/>
+      <c r="G67" s="9"/>
       <c r="H67" s="8"/>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>57</v>
       </c>
@@ -1515,7 +1564,7 @@
       <c r="G68" s="7"/>
       <c r="H68" s="5"/>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>58</v>
       </c>
@@ -1529,16 +1578,16 @@
       <c r="G69" s="7"/>
       <c r="H69" s="5"/>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B70" s="8"/>
       <c r="C70" s="8"/>
       <c r="D70" s="8"/>
       <c r="E70" s="8"/>
-      <c r="F70" s="10"/>
-      <c r="G70" s="10"/>
+      <c r="F70" s="9"/>
+      <c r="G70" s="9"/>
       <c r="H70" s="8"/>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>59</v>
       </c>
@@ -1558,7 +1607,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>60</v>
       </c>
@@ -1578,16 +1627,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B73" s="8"/>
       <c r="C73" s="8"/>
       <c r="D73" s="8"/>
       <c r="E73" s="8"/>
-      <c r="F73" s="10"/>
-      <c r="G73" s="10"/>
+      <c r="F73" s="9"/>
+      <c r="G73" s="9"/>
       <c r="H73" s="8"/>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>61</v>
       </c>
@@ -1601,7 +1650,7 @@
       <c r="G74" s="7"/>
       <c r="H74" s="5"/>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>62</v>
       </c>
@@ -1615,16 +1664,16 @@
       <c r="G75" s="7"/>
       <c r="H75" s="5"/>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B76" s="8"/>
       <c r="C76" s="8"/>
       <c r="D76" s="8"/>
       <c r="E76" s="8"/>
-      <c r="F76" s="10"/>
-      <c r="G76" s="10"/>
+      <c r="F76" s="9"/>
+      <c r="G76" s="9"/>
       <c r="H76" s="8"/>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>63</v>
       </c>
@@ -1655,24 +1704,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Je suis en vert en fait
</commit_message>
<xml_diff>
--- a/gestion-projet/Liste des taches.xlsx
+++ b/gestion-projet/Liste des taches.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19965" windowHeight="8640"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18780" windowHeight="7125"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -307,7 +307,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -364,12 +364,12 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
@@ -682,7 +682,7 @@
   <dimension ref="A1:J77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,15 +699,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
@@ -719,18 +719,18 @@
       <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J4" s="11" t="s">
+      <c r="J4" s="10" t="s">
         <v>66</v>
       </c>
     </row>
@@ -759,7 +759,7 @@
       <c r="H5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="11" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Début tache Classe Salle
</commit_message>
<xml_diff>
--- a/gestion-projet/Liste des taches.xlsx
+++ b/gestion-projet/Liste des taches.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="69">
   <si>
     <t>A faire</t>
   </si>
@@ -682,7 +682,7 @@
   <dimension ref="A1:J77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,7 +763,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J6" s="13" t="s">
         <v>68</v>
       </c>
@@ -852,13 +852,17 @@
       <c r="A17" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="7"/>
+      <c r="E17" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17" s="7">
+        <v>42640</v>
+      </c>
       <c r="G17" s="7"/>
       <c r="H17" s="5"/>
     </row>

</xml_diff>

<commit_message>
Modif liste des taches
</commit_message>
<xml_diff>
--- a/gestion-projet/Liste des taches.xlsx
+++ b/gestion-projet/Liste des taches.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18780" windowHeight="7125"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19965" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="69">
   <si>
     <t>A faire</t>
   </si>
@@ -368,10 +368,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -682,7 +682,7 @@
   <dimension ref="A1:J77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,15 +699,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
     </row>
     <row r="2" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
@@ -719,15 +719,15 @@
       <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J4" s="10" t="s">
@@ -764,7 +764,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J6" s="13" t="s">
+      <c r="J6" s="12" t="s">
         <v>68</v>
       </c>
     </row>
@@ -857,7 +857,9 @@
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
+      <c r="E17" s="10" t="s">
+        <v>66</v>
+      </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="5"/>

</xml_diff>